<commit_message>
Template Management & Send Message Tab Assertion update
</commit_message>
<xml_diff>
--- a/Excels/BulkUploadTemplate.xlsx
+++ b/Excels/BulkUploadTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Ticket Id</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>210321000129</t>
+  </si>
+  <si>
+    <t>210321000131</t>
+  </si>
+  <si>
+    <t>210321000132</t>
   </si>
 </sst>
 </file>
@@ -412,12 +418,12 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>